<commit_message>
String escape operators and Interpolations
</commit_message>
<xml_diff>
--- a/2024FEB_B6_Daily_Class.xlsx
+++ b/2024FEB_B6_Daily_Class.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCCSB6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9514789E-379A-4227-8C9E-E58D84EF1001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>S.N.</t>
   </si>
@@ -173,15 +179,21 @@
   </si>
   <si>
     <t>String manipulation</t>
+  </si>
+  <si>
+    <t>String Escape characters, String interpolation</t>
+  </si>
+  <si>
+    <t>Ram Nawami Holiday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode=",,"/>
-    <numFmt numFmtId="165" formatCode="dddd, mmmm dd, yyyy"/>
+    <numFmt numFmtId="164" formatCode="\,"/>
+    <numFmt numFmtId="165" formatCode="dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -214,11 +226,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFff0000"/>
+        <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -274,66 +286,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -344,10 +372,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -385,71 +413,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,7 +505,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -500,11 +528,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -513,13 +541,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -529,7 +557,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -538,7 +566,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -547,7 +575,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -555,10 +583,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -623,22 +651,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68:C94"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="28.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="90.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="4.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -660,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -671,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -682,7 +712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -693,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -704,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -715,7 +745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -726,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -737,7 +767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -748,7 +778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -759,7 +789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -770,7 +800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -781,7 +811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -792,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -803,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="8">
         <v>45347</v>
@@ -812,7 +842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="8">
         <v>45348</v>
@@ -821,7 +851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="8">
         <v>45349</v>
@@ -830,7 +860,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="8">
         <v>45350</v>
@@ -839,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="8">
         <v>45351</v>
@@ -848,7 +878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="8">
         <v>45352</v>
@@ -857,7 +887,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="8">
         <v>45353</v>
@@ -866,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="8">
         <v>45354</v>
@@ -875,7 +905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="8">
         <v>45355</v>
@@ -884,7 +914,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="8">
         <v>45356</v>
@@ -893,7 +923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="8">
         <v>45357</v>
@@ -902,7 +932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="8">
         <v>45358</v>
@@ -911,7 +941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="8">
         <v>45359</v>
@@ -920,7 +950,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="8">
         <v>45360</v>
@@ -929,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="8">
         <v>45361</v>
@@ -938,7 +968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="8">
         <v>45362</v>
@@ -947,7 +977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="8">
         <v>45363</v>
@@ -956,7 +986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="8">
         <v>45364</v>
@@ -965,7 +995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="8">
         <v>45365</v>
@@ -974,7 +1004,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row r="35" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="8">
         <v>45366</v>
@@ -983,7 +1013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="8">
         <v>45367</v>
@@ -992,7 +1022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="8">
         <v>45368</v>
@@ -1001,7 +1031,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="8">
         <v>45369</v>
@@ -1010,7 +1040,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="8">
         <v>45370</v>
@@ -1019,7 +1049,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="8">
         <v>45371</v>
@@ -1028,7 +1058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row r="41" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="8">
         <v>45372</v>
@@ -1037,7 +1067,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row r="42" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="8">
         <v>45373</v>
@@ -1046,7 +1076,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+    <row r="43" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="8">
         <v>45374</v>
@@ -1055,7 +1085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row r="44" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="8">
         <v>45375</v>
@@ -1064,7 +1094,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row r="45" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="8">
         <v>45376</v>
@@ -1073,7 +1103,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row r="46" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="8">
         <v>45377</v>
@@ -1082,7 +1112,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row r="47" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="8">
         <v>45378</v>
@@ -1091,7 +1121,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row r="48" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="12">
         <v>45379</v>
@@ -1100,7 +1130,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="12">
         <v>45380</v>
@@ -1109,7 +1139,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+    <row r="50" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="12">
         <v>45381</v>
@@ -1118,7 +1148,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row r="51" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="12">
         <v>45382</v>
@@ -1127,7 +1157,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row r="52" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="12">
         <v>45383</v>
@@ -1136,7 +1166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row r="53" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="12">
         <v>45384</v>
@@ -1145,7 +1175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row r="54" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="12">
         <v>45385</v>
@@ -1154,7 +1184,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+    <row r="55" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="12">
         <v>45386</v>
@@ -1163,7 +1193,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row r="56" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="12">
         <v>45387</v>
@@ -1172,7 +1202,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+    <row r="57" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="12">
         <v>45388</v>
@@ -1181,7 +1211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row r="58" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="12">
         <v>45389</v>
@@ -1190,7 +1220,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+    <row r="59" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="12">
         <v>45390</v>
@@ -1199,7 +1229,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row r="60" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="12">
         <v>45391</v>
@@ -1208,7 +1238,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+    <row r="61" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="12">
         <v>45392</v>
@@ -1217,7 +1247,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+    <row r="62" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="12">
         <v>45393</v>
@@ -1226,7 +1256,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+    <row r="63" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="12">
         <v>45394</v>
@@ -1235,7 +1265,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+    <row r="64" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="12">
         <v>45395</v>
@@ -1244,7 +1274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+    <row r="65" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="12">
         <v>45396</v>
@@ -1253,7 +1283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+    <row r="66" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="12">
         <v>45397</v>
@@ -1262,12 +1292,205 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="20.25">
+    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="12">
         <v>45398</v>
       </c>
-      <c r="C67" s="9"/>
+      <c r="C67" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="12">
+        <v>45399</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="12">
+        <v>45400</v>
+      </c>
+      <c r="C69" s="17"/>
+    </row>
+    <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="12">
+        <v>45401</v>
+      </c>
+      <c r="C70" s="17"/>
+    </row>
+    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="12">
+        <v>45402</v>
+      </c>
+      <c r="C71" s="17"/>
+    </row>
+    <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="12">
+        <v>45403</v>
+      </c>
+      <c r="C72" s="17"/>
+    </row>
+    <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="12">
+        <v>45404</v>
+      </c>
+      <c r="C73" s="17"/>
+    </row>
+    <row r="74" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="12">
+        <v>45405</v>
+      </c>
+      <c r="C74" s="17"/>
+    </row>
+    <row r="75" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="12">
+        <v>45406</v>
+      </c>
+      <c r="C75" s="17"/>
+    </row>
+    <row r="76" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="12">
+        <v>45407</v>
+      </c>
+      <c r="C76" s="17"/>
+    </row>
+    <row r="77" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+      <c r="B77" s="12">
+        <v>45408</v>
+      </c>
+      <c r="C77" s="17"/>
+    </row>
+    <row r="78" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="12">
+        <v>45409</v>
+      </c>
+      <c r="C78" s="17"/>
+    </row>
+    <row r="79" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="12">
+        <v>45410</v>
+      </c>
+      <c r="C79" s="17"/>
+    </row>
+    <row r="80" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+      <c r="B80" s="12">
+        <v>45411</v>
+      </c>
+      <c r="C80" s="17"/>
+    </row>
+    <row r="81" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="12">
+        <v>45412</v>
+      </c>
+      <c r="C81" s="17"/>
+    </row>
+    <row r="82" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="12">
+        <v>45413</v>
+      </c>
+      <c r="C82" s="17"/>
+    </row>
+    <row r="83" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
+      <c r="B83" s="12">
+        <v>45414</v>
+      </c>
+      <c r="C83" s="17"/>
+    </row>
+    <row r="84" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="13"/>
+      <c r="B84" s="12">
+        <v>45415</v>
+      </c>
+      <c r="C84" s="17"/>
+    </row>
+    <row r="85" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="12">
+        <v>45416</v>
+      </c>
+      <c r="C85" s="17"/>
+    </row>
+    <row r="86" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="13"/>
+      <c r="B86" s="12">
+        <v>45417</v>
+      </c>
+      <c r="C86" s="17"/>
+    </row>
+    <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+      <c r="B87" s="12">
+        <v>45418</v>
+      </c>
+      <c r="C87" s="17"/>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13"/>
+      <c r="B88" s="12">
+        <v>45419</v>
+      </c>
+      <c r="C88" s="17"/>
+    </row>
+    <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="13"/>
+      <c r="B89" s="12">
+        <v>45420</v>
+      </c>
+      <c r="C89" s="17"/>
+    </row>
+    <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="13"/>
+      <c r="B90" s="12">
+        <v>45421</v>
+      </c>
+      <c r="C90" s="17"/>
+    </row>
+    <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="13"/>
+      <c r="B91" s="12">
+        <v>45422</v>
+      </c>
+      <c r="C91" s="17"/>
+    </row>
+    <row r="92" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+      <c r="B92" s="12">
+        <v>45423</v>
+      </c>
+      <c r="C92" s="17"/>
+    </row>
+    <row r="93" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+      <c r="B93" s="12">
+        <v>45424</v>
+      </c>
+      <c r="C93" s="17"/>
+    </row>
+    <row r="94" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="13"/>
+      <c r="B94" s="12">
+        <v>45425</v>
+      </c>
+      <c r="C94" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>